<commit_message>
Fix league war bug
</commit_message>
<xml_diff>
--- a/const/league_const.xlsx
+++ b/const/league_const.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="100" windowWidth="25540" windowHeight="13520"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="25540" windowHeight="13520"/>
   </bookViews>
   <sheets>
     <sheet name="league" sheetId="2" r:id="rId1"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -644,10 +644,10 @@
         <v>100</v>
       </c>
       <c r="G4" s="1">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ref="I4:I17" si="0">D4*E4*24*1000/100</f>
@@ -695,11 +695,10 @@
         <v>100</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G18" si="1">F5*2</f>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="0"/>
@@ -747,11 +746,10 @@
         <v>100</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="0"/>
@@ -799,11 +797,10 @@
         <v>100</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
@@ -851,11 +848,10 @@
         <v>100</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="0"/>
@@ -903,11 +899,10 @@
         <v>100</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H9" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="0"/>
@@ -955,11 +950,10 @@
         <v>100</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="0"/>
@@ -1007,11 +1001,10 @@
         <v>100</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H11" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="0"/>
@@ -1059,11 +1052,10 @@
         <v>100</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H12" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="0"/>
@@ -1111,11 +1103,10 @@
         <v>100</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="0"/>
@@ -1163,11 +1154,10 @@
         <v>100</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H14" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="0"/>
@@ -1215,11 +1205,10 @@
         <v>100</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H15" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="0"/>
@@ -1267,11 +1256,10 @@
         <v>100</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I16" s="5">
         <v>1000</v>
@@ -1318,11 +1306,10 @@
         <v>100</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H17" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="0"/>
@@ -1370,14 +1357,13 @@
         <v>100</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H18" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" ref="I18" si="2">D18*E18*24*1000/100</f>
+        <f t="shared" ref="I18" si="1">D18*E18*24*1000/100</f>
         <v>1200</v>
       </c>
       <c r="J18" s="5">

</xml_diff>